<commit_message>
test: testing EXCEL reading
</commit_message>
<xml_diff>
--- a/config/node/backend/data/cennik.xlsx
+++ b/config/node/backend/data/cennik.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\StronaMonikaReact\config\node\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C92E619-F3A3-4496-BB2C-C6558A3D2F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DF384A-FCEB-4E4C-9EBA-E8CA72448F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4DB6F867-2552-414A-BFD2-AB60479A5D88}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Pedicure</t>
   </si>
@@ -57,6 +57,18 @@
   </si>
   <si>
     <t>eeeee</t>
+  </si>
+  <si>
+    <t>Botoks</t>
+  </si>
+  <si>
+    <t>Zabieg et</t>
+  </si>
+  <si>
+    <t>Oczyszczanie</t>
+  </si>
+  <si>
+    <t>Opis</t>
   </si>
 </sst>
 </file>
@@ -429,7 +441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3D7DE2-9127-49D9-96AA-B2504799E15F}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -470,6 +482,28 @@
         <v>300</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>500</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>